<commit_message>
Updated README with changes and added R script
</commit_message>
<xml_diff>
--- a/data/Inflation_Rates.xlsx
+++ b/data/Inflation_Rates.xlsx
@@ -1,75 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\humbl\OneDrive\Documents\R PROJECTS\Pension_Fund_Analysis\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>February</t>
-  </si>
-  <si>
-    <t>January</t>
-  </si>
-  <si>
-    <t>December</t>
-  </si>
-  <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>DATA ON INFLATION RATES FROM 
 JANUARY 2022 TO DECEMBER 2023</t>
   </si>
   <si>
-    <t>YEAR</t>
+    <t>12 MONTH INFLATION</t>
   </si>
   <si>
-    <t>MONTH</t>
-  </si>
-  <si>
-    <t>12-MONTH INFLATION</t>
+    <t>DATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,7 +372,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -540,17 +506,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -620,15 +575,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -639,6 +585,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -688,6 +643,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -734,7 +697,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -766,9 +729,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -800,6 +764,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -975,262 +940,229 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="5.140625" style="7"/>
+    <col min="1" max="1" width="22.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="5.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:3" s="4" customFormat="1">
-      <c r="A2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="5">
-        <v>2022</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>44562</v>
+      </c>
+      <c r="B3" s="3">
         <v>5.39</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6">
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>44593</v>
+      </c>
+      <c r="B4" s="3">
         <v>5.08</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="6">
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>44621</v>
+      </c>
+      <c r="B5" s="3">
         <v>5.56</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6">
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>44652</v>
+      </c>
+      <c r="B6" s="3">
         <v>6.47</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6">
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>44682</v>
+      </c>
+      <c r="B7" s="3">
         <v>7.08</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="6">
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>44713</v>
+      </c>
+      <c r="B8" s="3">
         <v>7.91</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="6">
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>44743</v>
+      </c>
+      <c r="B9" s="3">
         <v>8.32</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="6">
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>44774</v>
+      </c>
+      <c r="B10" s="3">
         <v>8.5299999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="6">
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>44805</v>
+      </c>
+      <c r="B11" s="3">
         <v>9.18</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="6">
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>44835</v>
+      </c>
+      <c r="B12" s="3">
         <v>9.59</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="6">
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>44866</v>
+      </c>
+      <c r="B13" s="3">
         <v>9.48</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="6">
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>44896</v>
+      </c>
+      <c r="B14" s="3">
         <v>9.06</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="5">
-        <v>2023</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="6">
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>44927</v>
+      </c>
+      <c r="B15" s="3">
         <v>8.98</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="6">
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>44958</v>
+      </c>
+      <c r="B16" s="3">
         <v>9.23</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="6">
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>44986</v>
+      </c>
+      <c r="B17" s="3">
         <v>9.19</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="6">
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>45017</v>
+      </c>
+      <c r="B18" s="3">
         <v>7.9</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="6">
+    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>45047</v>
+      </c>
+      <c r="B19" s="3">
         <v>8.0299999999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="6">
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>45078</v>
+      </c>
+      <c r="B20" s="3">
         <v>7.88</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="6">
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>45108</v>
+      </c>
+      <c r="B21" s="3">
         <v>7.28</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="6">
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>45139</v>
+      </c>
+      <c r="B22" s="3">
         <v>6.73</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="6">
+    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>45170</v>
+      </c>
+      <c r="B23" s="3">
         <v>6.78</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="6">
+    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>45200</v>
+      </c>
+      <c r="B24" s="3">
         <v>6.92</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="6">
+    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>45231</v>
+      </c>
+      <c r="B25" s="3">
         <v>6.8</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="6">
+    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>45261</v>
+      </c>
+      <c r="B26" s="3">
         <v>6.63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>